<commit_message>
Added a feature to perform regression on both components at the same time
</commit_message>
<xml_diff>
--- a/case3_Borate/_HCL_PCR642Ca.xlsx
+++ b/case3_Borate/_HCL_PCR642Ca.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\28820169\Downloads\BO Papers\Regression_Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\28820169\Downloads\BO_Papers\MEng_Code\case3_Borate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B089B3C-98E2-4F79-A473-3C43714599C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8553FFD-2A2F-4A05-AB98-3F1A320883B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,7 +51,7 @@
     Add the concentration data</t>
       </text>
     </comment>
-    <comment ref="U2" authorId="1" shapeId="0" xr:uid="{5AF1EB17-828D-47F0-A2E0-4DB30A2B1BE1}">
+    <comment ref="W2" authorId="1" shapeId="0" xr:uid="{5AF1EB17-828D-47F0-A2E0-4DB30A2B1BE1}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>g/l</t>
   </si>
@@ -231,9 +231,6 @@
     <t>Cl</t>
   </si>
   <si>
-    <t>mg/l</t>
-  </si>
-  <si>
     <t>Chloride</t>
   </si>
   <si>
@@ -253,6 +250,12 @@
   </si>
   <si>
     <t>F31</t>
+  </si>
+  <si>
+    <t>Borate mg/l</t>
+  </si>
+  <si>
+    <t>HCl mg/l</t>
   </si>
 </sst>
 </file>
@@ -466,7 +469,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -514,6 +517,9 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -726,7 +732,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>glucose!$G$2:$G$27</c:f>
+              <c:f>glucose!$I$2:$I$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
@@ -937,7 +943,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>glucose!$G$2:$G$27</c:f>
+              <c:f>glucose!$I$2:$I$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
@@ -1886,13 +1892,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>1158240</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>426720</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>167640</xdr:rowOff>
@@ -2195,7 +2201,7 @@
   <threadedComment ref="E2" dT="2025-05-21T11:39:01.54" personId="{75DC4CFE-A161-4013-83B8-642EC4E1C773}" id="{53FEF5DB-474A-44D0-A448-7BC243F78234}">
     <text>Add the concentration data</text>
   </threadedComment>
-  <threadedComment ref="U2" dT="2024-10-21T14:49:01.57" personId="{75DC4CFE-A161-4013-83B8-642EC4E1C773}" id="{5AF1EB17-828D-47F0-A2E0-4DB30A2B1BE1}">
+  <threadedComment ref="W2" dT="2024-10-21T14:49:01.57" personId="{75DC4CFE-A161-4013-83B8-642EC4E1C773}" id="{5AF1EB17-828D-47F0-A2E0-4DB30A2B1BE1}">
     <text>Get from isotherm reg</text>
   </threadedComment>
 </ThreadedComments>
@@ -2203,32 +2209,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U74"/>
+  <dimension ref="A1:W74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5546875" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="9.5546875" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>29</v>
       </c>
@@ -2242,58 +2248,62 @@
         <v>30</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="F1" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="O1" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="P1" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="Q1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="R1" s="24" t="s">
+      <c r="T1" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -2301,7 +2311,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="1">
-        <f t="shared" ref="C2:C27" si="0">B2*$J$5</f>
+        <f t="shared" ref="C2:C27" si="0">B2*$L$5</f>
         <v>0</v>
       </c>
       <c r="D2" s="1">
@@ -2311,61 +2321,63 @@
       <c r="E2" s="1">
         <v>0</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="8">
         <f>E2/1000</f>
         <v>0</v>
       </c>
-      <c r="G2" s="1">
-        <f>F3*(1/1000)</f>
+      <c r="I2" s="1">
+        <f>H3*(1/1000)</f>
         <v>5.5740000000000003E-6</v>
       </c>
-      <c r="H2" s="8">
+      <c r="J2" s="8">
         <f>8.4*0.0166666667</f>
         <v>0.14000000028000001</v>
       </c>
-      <c r="I2" s="8">
+      <c r="K2" s="8">
         <v>30</v>
       </c>
-      <c r="J2" s="8">
+      <c r="L2" s="8">
         <v>150</v>
       </c>
-      <c r="K2" s="1">
-        <f>I2/J2</f>
+      <c r="M2" s="1">
+        <f>K2/L2</f>
         <v>0.2</v>
       </c>
-      <c r="L2" s="10">
+      <c r="N2" s="10">
         <f>9.726/1000</f>
         <v>9.7260000000000003E-3</v>
       </c>
-      <c r="M2" s="9">
+      <c r="O2" s="9">
         <v>24</v>
       </c>
-      <c r="N2" s="11">
+      <c r="P2" s="11">
         <v>2</v>
       </c>
-      <c r="O2" s="11">
+      <c r="Q2" s="11">
         <v>0.4</v>
       </c>
-      <c r="P2" s="1">
+      <c r="R2" s="1">
         <v>60</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="R2" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="U2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="T2" s="1">
+      <c r="V2" s="1">
         <v>0</v>
       </c>
-      <c r="U2" s="1">
+      <c r="W2" s="1">
         <v>0.3</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2383,20 +2395,22 @@
       <c r="E3" s="22">
         <v>5.5739999999999998</v>
       </c>
-      <c r="F3" s="8">
-        <f t="shared" ref="F3:F33" si="2">E3/1000</f>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="8">
+        <f t="shared" ref="H3:H33" si="2">E3/1000</f>
         <v>5.574E-3</v>
       </c>
-      <c r="G3" s="1">
-        <f t="shared" ref="G3:G33" si="3">F4*(1/1000)</f>
+      <c r="I3" s="1">
+        <f t="shared" ref="I3:I33" si="3">H4*(1/1000)</f>
         <v>4.1269999999999996E-6</v>
       </c>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -2414,25 +2428,27 @@
       <c r="E4" s="22">
         <v>4.1269999999999998</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="8">
         <f t="shared" si="2"/>
         <v>4.1269999999999996E-3</v>
       </c>
-      <c r="G4" s="1">
+      <c r="I4" s="1">
         <f t="shared" si="3"/>
         <v>4.2569999999999992E-6</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="K4" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="J4" s="8">
+      <c r="L4" s="8">
         <v>36</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -2450,26 +2466,28 @@
       <c r="E5" s="22">
         <v>4.2569999999999997</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="8">
         <f t="shared" si="2"/>
         <v>4.2569999999999995E-3</v>
       </c>
-      <c r="G5" s="1">
+      <c r="I5" s="1">
         <f t="shared" si="3"/>
         <v>4.1830000000000004E-6</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="J5" s="1">
-        <f>J4/60</f>
+      <c r="L5" s="1">
+        <f>L4/60</f>
         <v>0.6</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -2487,16 +2505,18 @@
       <c r="E6" s="22">
         <v>4.1829999999999998</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="8">
         <f t="shared" si="2"/>
         <v>4.1830000000000001E-3</v>
       </c>
-      <c r="G6" s="1">
+      <c r="I6" s="1">
         <f t="shared" si="3"/>
         <v>3.4640000000000002E-6</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -2514,16 +2534,18 @@
       <c r="E7" s="22">
         <v>3.464</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="8">
         <f t="shared" si="2"/>
         <v>3.4640000000000001E-3</v>
       </c>
-      <c r="G7" s="1">
+      <c r="I7" s="1">
         <f t="shared" si="3"/>
         <v>4.0450000000000002E-6</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -2541,17 +2563,19 @@
       <c r="E8" s="22">
         <v>4.0449999999999999</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="8">
         <f t="shared" si="2"/>
         <v>4.045E-3</v>
       </c>
-      <c r="G8" s="1">
+      <c r="I8" s="1">
         <f t="shared" si="3"/>
         <v>4.0820000000000001E-6</v>
       </c>
-      <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2569,17 +2593,19 @@
       <c r="E9" s="22">
         <v>4.0819999999999999</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="8">
         <f t="shared" si="2"/>
         <v>4.0819999999999997E-3</v>
       </c>
-      <c r="G9" s="1">
+      <c r="I9" s="1">
         <f t="shared" si="3"/>
         <v>3.8639999999999998E-6</v>
       </c>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -2597,17 +2623,19 @@
       <c r="E10" s="22">
         <v>3.8639999999999999</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="8">
         <f t="shared" si="2"/>
         <v>3.8639999999999998E-3</v>
       </c>
-      <c r="G10" s="1">
+      <c r="I10" s="1">
         <f t="shared" si="3"/>
         <v>3.827E-6</v>
       </c>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -2625,16 +2653,18 @@
       <c r="E11" s="22">
         <v>3.827</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="8">
         <f t="shared" si="2"/>
         <v>3.8270000000000001E-3</v>
       </c>
-      <c r="G11" s="1">
+      <c r="I11" s="1">
         <f t="shared" si="3"/>
         <v>1.1164999999999999E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -2652,17 +2682,19 @@
       <c r="E12" s="22">
         <v>11.164999999999999</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="8">
         <f t="shared" si="2"/>
         <v>1.1165E-2</v>
       </c>
-      <c r="G12" s="1">
+      <c r="I12" s="1">
         <f t="shared" si="3"/>
         <v>1.2213800000000002E-4</v>
       </c>
-      <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -2680,17 +2712,19 @@
       <c r="E13" s="22">
         <v>122.13800000000001</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="8">
         <f t="shared" si="2"/>
         <v>0.12213800000000001</v>
       </c>
-      <c r="G13" s="1">
+      <c r="I13" s="1">
         <f t="shared" si="3"/>
         <v>5.8123599999999995E-4</v>
       </c>
-      <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -2708,17 +2742,19 @@
       <c r="E14" s="22">
         <v>581.23599999999999</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="8">
         <f t="shared" si="2"/>
         <v>0.58123599999999997</v>
       </c>
-      <c r="G14" s="1">
+      <c r="I14" s="1">
         <f t="shared" si="3"/>
         <v>6.9794300000000002E-4</v>
       </c>
-      <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="J14" s="2"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -2736,17 +2772,19 @@
       <c r="E15" s="22">
         <v>697.94299999999998</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="8">
         <f t="shared" si="2"/>
         <v>0.69794299999999998</v>
       </c>
-      <c r="G15" s="1">
+      <c r="I15" s="1">
         <f t="shared" si="3"/>
         <v>1.4288009999999999E-3</v>
       </c>
-      <c r="H15" s="2"/>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="J15" s="2"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -2764,17 +2802,19 @@
       <c r="E16" s="22">
         <v>1428.8009999999999</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="8">
         <f t="shared" si="2"/>
         <v>1.428801</v>
       </c>
-      <c r="G16" s="1">
+      <c r="I16" s="1">
         <f t="shared" si="3"/>
         <v>1.272979E-3</v>
       </c>
-      <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J16" s="2"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -2792,17 +2832,19 @@
       <c r="E17" s="22">
         <v>1272.979</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="8">
         <f t="shared" si="2"/>
         <v>1.2729790000000001</v>
       </c>
-      <c r="G17" s="1">
+      <c r="I17" s="1">
         <f t="shared" si="3"/>
         <v>1.434137E-3</v>
       </c>
-      <c r="H17" s="2"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J17" s="2"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -2820,17 +2862,19 @@
       <c r="E18" s="22">
         <v>1434.1369999999999</v>
       </c>
-      <c r="F18" s="8">
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="8">
         <f t="shared" si="2"/>
         <v>1.434137</v>
       </c>
-      <c r="G18" s="1">
+      <c r="I18" s="1">
         <f t="shared" si="3"/>
         <v>1.3246710000000001E-3</v>
       </c>
-      <c r="H18" s="2"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J18" s="2"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -2848,17 +2892,19 @@
       <c r="E19" s="22">
         <v>1324.671</v>
       </c>
-      <c r="F19" s="8">
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="8">
         <f t="shared" si="2"/>
         <v>1.3246710000000002</v>
       </c>
-      <c r="G19" s="1">
+      <c r="I19" s="1">
         <f t="shared" si="3"/>
         <v>9.1704799999999995E-4</v>
       </c>
-      <c r="H19" s="2"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J19" s="2"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -2876,17 +2922,19 @@
       <c r="E20" s="22">
         <v>917.048</v>
       </c>
-      <c r="F20" s="8">
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="8">
         <f t="shared" si="2"/>
         <v>0.91704799999999997</v>
       </c>
-      <c r="G20" s="1">
+      <c r="I20" s="1">
         <f t="shared" si="3"/>
         <v>6.3300699999999999E-4</v>
       </c>
-      <c r="H20" s="2"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J20" s="2"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -2904,17 +2952,19 @@
       <c r="E21" s="22">
         <v>633.00699999999995</v>
       </c>
-      <c r="F21" s="8">
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="8">
         <f t="shared" si="2"/>
         <v>0.63300699999999999</v>
       </c>
-      <c r="G21" s="1">
+      <c r="I21" s="1">
         <f t="shared" si="3"/>
         <v>3.05975E-4</v>
       </c>
-      <c r="H21" s="2"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J21" s="2"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -2932,17 +2982,19 @@
       <c r="E22" s="22">
         <v>305.97500000000002</v>
       </c>
-      <c r="F22" s="8">
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="8">
         <f t="shared" si="2"/>
         <v>0.305975</v>
       </c>
-      <c r="G22" s="1">
+      <c r="I22" s="1">
         <f t="shared" si="3"/>
         <v>1.20835E-4</v>
       </c>
-      <c r="H22" s="2"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J22" s="2"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -2960,17 +3012,19 @@
       <c r="E23" s="22">
         <v>120.83499999999999</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="8">
         <f t="shared" si="2"/>
         <v>0.120835</v>
       </c>
-      <c r="G23" s="1">
+      <c r="I23" s="1">
         <f t="shared" si="3"/>
         <v>3.9109999999999997E-5</v>
       </c>
-      <c r="H23" s="2"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J23" s="2"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -2988,17 +3042,19 @@
       <c r="E24" s="22">
         <v>39.11</v>
       </c>
-      <c r="F24" s="8">
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="8">
         <f t="shared" si="2"/>
         <v>3.9109999999999999E-2</v>
       </c>
-      <c r="G24" s="1">
+      <c r="I24" s="1">
         <f t="shared" si="3"/>
         <v>1.5946999999999998E-5</v>
       </c>
-      <c r="H24" s="2"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J24" s="2"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -3016,17 +3072,19 @@
       <c r="E25" s="22">
         <v>15.946999999999999</v>
       </c>
-      <c r="F25" s="8">
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="8">
         <f t="shared" si="2"/>
         <v>1.5946999999999999E-2</v>
       </c>
-      <c r="G25" s="1">
+      <c r="I25" s="1">
         <f t="shared" si="3"/>
         <v>7.9260000000000017E-6</v>
       </c>
-      <c r="H25" s="2"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J25" s="2"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -3044,17 +3102,19 @@
       <c r="E26" s="22">
         <v>7.9260000000000002</v>
       </c>
-      <c r="F26" s="8">
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="8">
         <f t="shared" si="2"/>
         <v>7.9260000000000008E-3</v>
       </c>
-      <c r="G26" s="1">
+      <c r="I26" s="1">
         <f t="shared" si="3"/>
         <v>5.5690000000000004E-6</v>
       </c>
-      <c r="H26" s="2"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J26" s="2"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>25</v>
       </c>
@@ -3072,25 +3132,27 @@
       <c r="E27" s="22">
         <v>5.569</v>
       </c>
-      <c r="F27" s="8">
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="8">
         <f t="shared" si="2"/>
         <v>5.5690000000000002E-3</v>
       </c>
-      <c r="G27" s="1">
+      <c r="I27" s="1">
         <f t="shared" si="3"/>
         <v>4.5750000000000002E-6</v>
       </c>
-      <c r="H27" s="2"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J27" s="2"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B28" s="1">
         <v>26</v>
       </c>
       <c r="C28" s="1">
-        <f t="shared" ref="C28:C33" si="4">B28*$J$5</f>
+        <f t="shared" ref="C28:C33" si="4">B28*$L$5</f>
         <v>15.6</v>
       </c>
       <c r="D28" s="1">
@@ -3100,18 +3162,20 @@
       <c r="E28" s="22">
         <v>4.5750000000000002</v>
       </c>
-      <c r="F28" s="8">
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="8">
         <f t="shared" si="2"/>
         <v>4.5750000000000001E-3</v>
       </c>
-      <c r="G28" s="1">
+      <c r="I28" s="1">
         <f t="shared" si="3"/>
         <v>4.8100000000000005E-6</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B29" s="1">
         <v>27</v>
@@ -3127,18 +3191,20 @@
       <c r="E29" s="22">
         <v>4.8099999999999996</v>
       </c>
-      <c r="F29" s="8">
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="8">
         <f t="shared" si="2"/>
         <v>4.81E-3</v>
       </c>
-      <c r="G29" s="1">
+      <c r="I29" s="1">
         <f t="shared" si="3"/>
         <v>4.9230000000000001E-6</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B30" s="1">
         <v>28</v>
@@ -3154,18 +3220,20 @@
       <c r="E30" s="22">
         <v>4.923</v>
       </c>
-      <c r="F30" s="8">
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="8">
         <f t="shared" si="2"/>
         <v>4.9230000000000003E-3</v>
       </c>
-      <c r="G30" s="1">
+      <c r="I30" s="1">
         <f t="shared" si="3"/>
         <v>3.5880000000000002E-5</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B31" s="1">
         <v>29</v>
@@ -3181,18 +3249,20 @@
       <c r="E31" s="22">
         <v>35.880000000000003</v>
       </c>
-      <c r="F31" s="8">
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="8">
         <f t="shared" si="2"/>
         <v>3.5880000000000002E-2</v>
       </c>
-      <c r="G31" s="1">
+      <c r="I31" s="1">
         <f t="shared" si="3"/>
         <v>3.6410000000000004E-6</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B32" s="1">
         <v>30</v>
@@ -3208,18 +3278,20 @@
       <c r="E32" s="22">
         <v>3.641</v>
       </c>
-      <c r="F32" s="8">
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="8">
         <f t="shared" si="2"/>
         <v>3.6410000000000001E-3</v>
       </c>
-      <c r="G32" s="1">
+      <c r="I32" s="1">
         <f t="shared" si="3"/>
         <v>4.1160000000000001E-6</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B33" s="1">
         <v>31</v>
@@ -3235,178 +3307,262 @@
       <c r="E33" s="23">
         <v>4.1159999999999997</v>
       </c>
-      <c r="F33" s="8">
+      <c r="F33" s="25"/>
+      <c r="G33" s="25"/>
+      <c r="H33" s="8">
         <f t="shared" si="2"/>
         <v>4.1159999999999999E-3</v>
       </c>
-      <c r="G33" s="1">
+      <c r="I33" s="1">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
-    </row>
-    <row r="49" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
+    </row>
+    <row r="49" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E49" s="6"/>
       <c r="F49" s="6"/>
-    </row>
-    <row r="50" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
+    </row>
+    <row r="50" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
-    </row>
-    <row r="51" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="G50" s="6"/>
+      <c r="H50" s="6"/>
+    </row>
+    <row r="51" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E51" s="7"/>
       <c r="F51" s="7"/>
-    </row>
-    <row r="52" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="G51" s="7"/>
+      <c r="H51" s="7"/>
+    </row>
+    <row r="52" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E52" s="7"/>
       <c r="F52" s="7"/>
-    </row>
-    <row r="53" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="G52" s="7"/>
+      <c r="H52" s="7"/>
+    </row>
+    <row r="53" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E53" s="7"/>
       <c r="F53" s="7"/>
-    </row>
-    <row r="54" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="G53" s="7"/>
+      <c r="H53" s="7"/>
+    </row>
+    <row r="54" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E54" s="7"/>
       <c r="F54" s="7"/>
-    </row>
-    <row r="55" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="G54" s="7"/>
+      <c r="H54" s="7"/>
+    </row>
+    <row r="55" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E55" s="7"/>
       <c r="F55" s="7"/>
-    </row>
-    <row r="56" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="G55" s="7"/>
+      <c r="H55" s="7"/>
+    </row>
+    <row r="56" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E56" s="7"/>
       <c r="F56" s="7"/>
-    </row>
-    <row r="57" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="G56" s="7"/>
+      <c r="H56" s="7"/>
+    </row>
+    <row r="57" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E57" s="7"/>
       <c r="F57" s="7"/>
-    </row>
-    <row r="58" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="G57" s="7"/>
+      <c r="H57" s="7"/>
+    </row>
+    <row r="58" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E58" s="7"/>
       <c r="F58" s="7"/>
-    </row>
-    <row r="59" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="G58" s="7"/>
+      <c r="H58" s="7"/>
+    </row>
+    <row r="59" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E59" s="7"/>
       <c r="F59" s="7"/>
-    </row>
-    <row r="60" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="G59" s="7"/>
+      <c r="H59" s="7"/>
+    </row>
+    <row r="60" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E60" s="7"/>
       <c r="F60" s="7"/>
-    </row>
-    <row r="61" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="G60" s="7"/>
+      <c r="H60" s="7"/>
+    </row>
+    <row r="61" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E61" s="7"/>
       <c r="F61" s="7"/>
-    </row>
-    <row r="62" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="G61" s="7"/>
+      <c r="H61" s="7"/>
+    </row>
+    <row r="62" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E62" s="7"/>
       <c r="F62" s="7"/>
-    </row>
-    <row r="63" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="G62" s="7"/>
+      <c r="H62" s="7"/>
+    </row>
+    <row r="63" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E63" s="7"/>
       <c r="F63" s="7"/>
-    </row>
-    <row r="64" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="G63" s="7"/>
+      <c r="H63" s="7"/>
+    </row>
+    <row r="64" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E64" s="7"/>
       <c r="F64" s="7"/>
-    </row>
-    <row r="65" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="G64" s="7"/>
+      <c r="H64" s="7"/>
+    </row>
+    <row r="65" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E65" s="7"/>
       <c r="F65" s="7"/>
-    </row>
-    <row r="66" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="G65" s="7"/>
+      <c r="H65" s="7"/>
+    </row>
+    <row r="66" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E66" s="7"/>
       <c r="F66" s="7"/>
-    </row>
-    <row r="67" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="G66" s="7"/>
+      <c r="H66" s="7"/>
+    </row>
+    <row r="67" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E67" s="7"/>
       <c r="F67" s="7"/>
-    </row>
-    <row r="68" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="G67" s="7"/>
+      <c r="H67" s="7"/>
+    </row>
+    <row r="68" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E68" s="7"/>
       <c r="F68" s="7"/>
-    </row>
-    <row r="69" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="G68" s="7"/>
+      <c r="H68" s="7"/>
+    </row>
+    <row r="69" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E69" s="7"/>
       <c r="F69" s="7"/>
-    </row>
-    <row r="70" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="G69" s="7"/>
+      <c r="H69" s="7"/>
+    </row>
+    <row r="70" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E70" s="7"/>
       <c r="F70" s="7"/>
-    </row>
-    <row r="71" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="G70" s="7"/>
+      <c r="H70" s="7"/>
+    </row>
+    <row r="71" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E71" s="7"/>
       <c r="F71" s="7"/>
-    </row>
-    <row r="72" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="G71" s="7"/>
+      <c r="H71" s="7"/>
+    </row>
+    <row r="72" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E72" s="7"/>
       <c r="F72" s="7"/>
-    </row>
-    <row r="73" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="G72" s="7"/>
+      <c r="H72" s="7"/>
+    </row>
+    <row r="73" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E73" s="7"/>
       <c r="F73" s="7"/>
-    </row>
-    <row r="74" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="G73" s="7"/>
+      <c r="H73" s="7"/>
+    </row>
+    <row r="74" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E74" s="7"/>
       <c r="F74" s="7"/>
+      <c r="G74" s="7"/>
+      <c r="H74" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -3786,6 +3942,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010048117A934AEAC441AF47E945F1AED0C0" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7272456f5b53c8ae1c345851aef95d27">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c39f1452-4462-4979-941b-c1317cfd14ce" xmlns:ns3="60199b31-2299-4531-8872-a3eaba744cbd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="16ed4d68a838bfbb08a7468a1792fb8f" ns2:_="" ns3:_="">
     <xsd:import namespace="c39f1452-4462-4979-941b-c1317cfd14ce"/>
@@ -4042,16 +4207,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21AAFDFA-AF70-4552-A086-9BCC58150335}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF42137A-B7F2-4A60-BAD9-4B8683F12BBF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4068,12 +4232,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21AAFDFA-AF70-4552-A086-9BCC58150335}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Make distinction betweenthe appropirete files for regression on coupled isoherms and uncoupled itoherms
</commit_message>
<xml_diff>
--- a/case3_Borate/_HCL_PCR642Ca.xlsx
+++ b/case3_Borate/_HCL_PCR642Ca.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\28820169\Downloads\BO_Papers\MEng_Code\case3_Borate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8553FFD-2A2F-4A05-AB98-3F1A320883B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{924C248C-A426-45F2-9895-042A3D0D50C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,7 +51,7 @@
     Add the concentration data</t>
       </text>
     </comment>
-    <comment ref="W2" authorId="1" shapeId="0" xr:uid="{5AF1EB17-828D-47F0-A2E0-4DB30A2B1BE1}">
+    <comment ref="U2" authorId="1" shapeId="0" xr:uid="{5AF1EB17-828D-47F0-A2E0-4DB30A2B1BE1}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>g/l</t>
   </si>
@@ -231,9 +231,6 @@
     <t>Cl</t>
   </si>
   <si>
-    <t>Chloride</t>
-  </si>
-  <si>
     <t>F26</t>
   </si>
   <si>
@@ -255,7 +252,7 @@
     <t>Borate mg/l</t>
   </si>
   <si>
-    <t>HCl mg/l</t>
+    <t>HCl</t>
   </si>
 </sst>
 </file>
@@ -509,17 +506,13 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -732,7 +725,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>glucose!$I$2:$I$27</c:f>
+              <c:f>glucose!$G$2:$G$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
@@ -943,7 +936,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>glucose!$I$2:$I$27</c:f>
+              <c:f>glucose!$G$2:$G$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
@@ -1892,13 +1885,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>1158240</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>426720</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>167640</xdr:rowOff>
@@ -2201,7 +2194,7 @@
   <threadedComment ref="E2" dT="2025-05-21T11:39:01.54" personId="{75DC4CFE-A161-4013-83B8-642EC4E1C773}" id="{53FEF5DB-474A-44D0-A448-7BC243F78234}">
     <text>Add the concentration data</text>
   </threadedComment>
-  <threadedComment ref="W2" dT="2024-10-21T14:49:01.57" personId="{75DC4CFE-A161-4013-83B8-642EC4E1C773}" id="{5AF1EB17-828D-47F0-A2E0-4DB30A2B1BE1}">
+  <threadedComment ref="U2" dT="2024-10-21T14:49:01.57" personId="{75DC4CFE-A161-4013-83B8-642EC4E1C773}" id="{5AF1EB17-828D-47F0-A2E0-4DB30A2B1BE1}">
     <text>Get from isotherm reg</text>
   </threadedComment>
 </ThreadedComments>
@@ -2209,10 +2202,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W74"/>
+  <dimension ref="A1:U74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2220,8 +2213,10 @@
     <col min="1" max="1" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="9.5546875" customWidth="1"/>
-    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5546875" customWidth="1"/>
+    <col min="9" max="9" width="36.77734375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="36.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.5546875" bestFit="1" customWidth="1"/>
@@ -2234,11 +2229,11 @@
     <col min="22" max="23" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="21" t="s">
         <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -2248,177 +2243,169 @@
         <v>30</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F1" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="H1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>44</v>
+      </c>
       <c r="J1" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>40</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="P1" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="Q1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R1" s="21" t="s">
+        <v>36</v>
+      </c>
       <c r="S1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="T1" s="24" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="W1" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="21">
         <v>0</v>
       </c>
       <c r="C2" s="1">
-        <f t="shared" ref="C2:C27" si="0">B2*$L$5</f>
+        <f>B2*$J$5</f>
         <v>0</v>
       </c>
       <c r="D2" s="1">
         <f>C2*60</f>
         <v>0</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="8">
         <v>0</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="8">
+      <c r="F2" s="23">
         <f>E2/1000</f>
         <v>0</v>
       </c>
-      <c r="I2" s="1">
-        <f>H3*(1/1000)</f>
+      <c r="G2" s="1">
+        <f>F3*(1/1000)</f>
         <v>5.5740000000000003E-6</v>
       </c>
-      <c r="J2" s="8">
+      <c r="H2" s="8">
         <f>8.4*0.0166666667</f>
         <v>0.14000000028000001</v>
       </c>
-      <c r="K2" s="8">
+      <c r="I2" s="8">
         <v>30</v>
       </c>
-      <c r="L2" s="8">
+      <c r="J2" s="8">
         <v>150</v>
       </c>
-      <c r="M2" s="1">
-        <f>K2/L2</f>
+      <c r="K2" s="1">
+        <f>I2/J2</f>
         <v>0.2</v>
       </c>
-      <c r="N2" s="10">
+      <c r="L2" s="10">
         <f>9.726/1000</f>
         <v>9.7260000000000003E-3</v>
       </c>
-      <c r="O2" s="9">
+      <c r="M2" s="9">
         <v>24</v>
       </c>
-      <c r="P2" s="11">
+      <c r="N2" s="11">
         <v>2</v>
       </c>
-      <c r="Q2" s="11">
+      <c r="O2" s="11">
         <v>0.4</v>
       </c>
-      <c r="R2" s="1">
+      <c r="P2" s="1">
         <v>60</v>
       </c>
+      <c r="Q2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R2" s="21" t="s">
+        <v>62</v>
+      </c>
       <c r="S2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="T2" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="U2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="V2" s="1">
+      <c r="T2" s="1">
         <v>0</v>
       </c>
-      <c r="W2" s="1">
+      <c r="U2" s="1">
         <v>0.3</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="21">
         <v>1</v>
       </c>
       <c r="C3" s="1">
-        <f t="shared" si="0"/>
+        <f>B3*$J$5</f>
         <v>0.6</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D27" si="1">C3*60</f>
+        <f t="shared" ref="D3:D27" si="0">C3*60</f>
         <v>36</v>
       </c>
       <c r="E3" s="22">
         <v>5.5739999999999998</v>
       </c>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="8">
-        <f t="shared" ref="H3:H33" si="2">E3/1000</f>
+      <c r="F3" s="23">
+        <f>E3/1000</f>
         <v>5.574E-3</v>
       </c>
-      <c r="I3" s="1">
-        <f t="shared" ref="I3:I33" si="3">H4*(1/1000)</f>
+      <c r="G3" s="1">
+        <f t="shared" ref="G3:G33" si="1">F4*(1/1000)</f>
         <v>4.1269999999999996E-6</v>
       </c>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A4" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="21">
         <v>2</v>
       </c>
       <c r="C4" s="1">
-        <f t="shared" si="0"/>
+        <f>B4*$J$5</f>
         <v>1.2</v>
       </c>
       <c r="D4" s="1">
@@ -2428,222 +2415,208 @@
       <c r="E4" s="22">
         <v>4.1269999999999998</v>
       </c>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="8">
-        <f t="shared" si="2"/>
+      <c r="F4" s="23">
+        <f>E4/1000</f>
         <v>4.1269999999999996E-3</v>
       </c>
-      <c r="I4" s="1">
-        <f t="shared" si="3"/>
+      <c r="G4" s="1">
+        <f t="shared" si="1"/>
         <v>4.2569999999999992E-6</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="I4" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="L4" s="8">
+      <c r="J4" s="8">
         <v>36</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="K4" s="21" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A5" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="21">
         <v>3</v>
       </c>
       <c r="C5" s="1">
+        <f>B5*$J$5</f>
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="D5" s="1">
         <f t="shared" si="0"/>
-        <v>1.7999999999999998</v>
-      </c>
-      <c r="D5" s="1">
-        <f t="shared" si="1"/>
         <v>107.99999999999999</v>
       </c>
       <c r="E5" s="22">
         <v>4.2569999999999997</v>
       </c>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="8">
-        <f t="shared" si="2"/>
+      <c r="F5" s="23">
+        <f>E5/1000</f>
         <v>4.2569999999999995E-3</v>
       </c>
-      <c r="I5" s="1">
-        <f t="shared" si="3"/>
+      <c r="G5" s="1">
+        <f t="shared" si="1"/>
         <v>4.1830000000000004E-6</v>
       </c>
+      <c r="I5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J5" s="1">
+        <f>J4/60</f>
+        <v>0.6</v>
+      </c>
       <c r="K5" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="L5" s="1">
-        <f>L4/60</f>
-        <v>0.6</v>
-      </c>
-      <c r="M5" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A6" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="21">
         <v>4</v>
       </c>
       <c r="C6" s="1">
+        <f>B6*$J$5</f>
+        <v>2.4</v>
+      </c>
+      <c r="D6" s="1">
         <f t="shared" si="0"/>
-        <v>2.4</v>
-      </c>
-      <c r="D6" s="1">
-        <f t="shared" si="1"/>
         <v>144</v>
       </c>
       <c r="E6" s="22">
         <v>4.1829999999999998</v>
       </c>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="8">
-        <f t="shared" si="2"/>
+      <c r="F6" s="23">
+        <f>E6/1000</f>
         <v>4.1830000000000001E-3</v>
       </c>
-      <c r="I6" s="1">
-        <f t="shared" si="3"/>
+      <c r="G6" s="1">
+        <f t="shared" si="1"/>
         <v>3.4640000000000002E-6</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A7" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="21">
         <v>5</v>
       </c>
       <c r="C7" s="1">
+        <f>B7*$J$5</f>
+        <v>3</v>
+      </c>
+      <c r="D7" s="1">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="D7" s="1">
-        <f t="shared" si="1"/>
         <v>180</v>
       </c>
       <c r="E7" s="22">
         <v>3.464</v>
       </c>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="8">
-        <f t="shared" si="2"/>
+      <c r="F7" s="23">
+        <f>E7/1000</f>
         <v>3.4640000000000001E-3</v>
       </c>
-      <c r="I7" s="1">
-        <f t="shared" si="3"/>
+      <c r="G7" s="1">
+        <f t="shared" si="1"/>
         <v>4.0450000000000002E-6</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A8" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="21">
         <v>6</v>
       </c>
       <c r="C8" s="1">
+        <f>B8*$J$5</f>
+        <v>3.5999999999999996</v>
+      </c>
+      <c r="D8" s="1">
         <f t="shared" si="0"/>
-        <v>3.5999999999999996</v>
-      </c>
-      <c r="D8" s="1">
-        <f t="shared" si="1"/>
         <v>215.99999999999997</v>
       </c>
       <c r="E8" s="22">
         <v>4.0449999999999999</v>
       </c>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="8">
-        <f t="shared" si="2"/>
+      <c r="F8" s="23">
+        <f>E8/1000</f>
         <v>4.045E-3</v>
       </c>
-      <c r="I8" s="1">
-        <f t="shared" si="3"/>
+      <c r="G8" s="1">
+        <f t="shared" si="1"/>
         <v>4.0820000000000001E-6</v>
       </c>
-      <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A9" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="21">
         <v>7</v>
       </c>
       <c r="C9" s="1">
+        <f>B9*$J$5</f>
+        <v>4.2</v>
+      </c>
+      <c r="D9" s="1">
         <f t="shared" si="0"/>
-        <v>4.2</v>
-      </c>
-      <c r="D9" s="1">
-        <f t="shared" si="1"/>
         <v>252</v>
       </c>
       <c r="E9" s="22">
         <v>4.0819999999999999</v>
       </c>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="8">
-        <f t="shared" si="2"/>
+      <c r="F9" s="23">
+        <f>E9/1000</f>
         <v>4.0819999999999997E-3</v>
       </c>
-      <c r="I9" s="1">
-        <f t="shared" si="3"/>
+      <c r="G9" s="1">
+        <f t="shared" si="1"/>
         <v>3.8639999999999998E-6</v>
       </c>
-      <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A10" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="21">
         <v>8</v>
       </c>
       <c r="C10" s="1">
+        <f>B10*$J$5</f>
+        <v>4.8</v>
+      </c>
+      <c r="D10" s="1">
         <f t="shared" si="0"/>
-        <v>4.8</v>
-      </c>
-      <c r="D10" s="1">
-        <f t="shared" si="1"/>
         <v>288</v>
       </c>
       <c r="E10" s="22">
         <v>3.8639999999999999</v>
       </c>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="8">
-        <f t="shared" si="2"/>
+      <c r="F10" s="23">
+        <f>E10/1000</f>
         <v>3.8639999999999998E-3</v>
       </c>
-      <c r="I10" s="1">
-        <f t="shared" si="3"/>
+      <c r="G10" s="1">
+        <f t="shared" si="1"/>
         <v>3.827E-6</v>
       </c>
-      <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A11" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="21">
         <v>9</v>
       </c>
       <c r="C11" s="1">
-        <f t="shared" si="0"/>
+        <f>B11*$J$5</f>
         <v>5.3999999999999995</v>
       </c>
       <c r="D11" s="1">
@@ -2653,760 +2626,684 @@
       <c r="E11" s="22">
         <v>3.827</v>
       </c>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="8">
-        <f t="shared" si="2"/>
+      <c r="F11" s="23">
+        <f>E11/1000</f>
         <v>3.8270000000000001E-3</v>
       </c>
-      <c r="I11" s="1">
-        <f t="shared" si="3"/>
+      <c r="G11" s="1">
+        <f t="shared" si="1"/>
         <v>1.1164999999999999E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A12" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="21">
         <v>10</v>
       </c>
       <c r="C12" s="1">
+        <f>B12*$J$5</f>
+        <v>6</v>
+      </c>
+      <c r="D12" s="1">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="D12" s="1">
-        <f t="shared" si="1"/>
         <v>360</v>
       </c>
       <c r="E12" s="22">
         <v>11.164999999999999</v>
       </c>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="8">
-        <f t="shared" si="2"/>
+      <c r="F12" s="23">
+        <f>E12/1000</f>
         <v>1.1165E-2</v>
       </c>
-      <c r="I12" s="1">
-        <f t="shared" si="3"/>
+      <c r="G12" s="1">
+        <f t="shared" si="1"/>
         <v>1.2213800000000002E-4</v>
       </c>
-      <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A13" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="21">
         <v>11</v>
       </c>
       <c r="C13" s="1">
+        <f>B13*$J$5</f>
+        <v>6.6</v>
+      </c>
+      <c r="D13" s="1">
         <f t="shared" si="0"/>
-        <v>6.6</v>
-      </c>
-      <c r="D13" s="1">
-        <f t="shared" si="1"/>
         <v>396</v>
       </c>
       <c r="E13" s="22">
         <v>122.13800000000001</v>
       </c>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="8">
-        <f t="shared" si="2"/>
+      <c r="F13" s="23">
+        <f>E13/1000</f>
         <v>0.12213800000000001</v>
       </c>
-      <c r="I13" s="1">
-        <f t="shared" si="3"/>
+      <c r="G13" s="1">
+        <f t="shared" si="1"/>
         <v>5.8123599999999995E-4</v>
       </c>
-      <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A14" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="21">
         <v>12</v>
       </c>
       <c r="C14" s="1">
+        <f>B14*$J$5</f>
+        <v>7.1999999999999993</v>
+      </c>
+      <c r="D14" s="1">
         <f t="shared" si="0"/>
-        <v>7.1999999999999993</v>
-      </c>
-      <c r="D14" s="1">
-        <f t="shared" si="1"/>
         <v>431.99999999999994</v>
       </c>
       <c r="E14" s="22">
         <v>581.23599999999999</v>
       </c>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="8">
-        <f t="shared" si="2"/>
+      <c r="F14" s="23">
+        <f>E14/1000</f>
         <v>0.58123599999999997</v>
       </c>
-      <c r="I14" s="1">
-        <f t="shared" si="3"/>
+      <c r="G14" s="1">
+        <f t="shared" si="1"/>
         <v>6.9794300000000002E-4</v>
       </c>
-      <c r="J14" s="2"/>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A15" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="21">
         <v>13</v>
       </c>
       <c r="C15" s="1">
+        <f>B15*$J$5</f>
+        <v>7.8</v>
+      </c>
+      <c r="D15" s="1">
         <f t="shared" si="0"/>
-        <v>7.8</v>
-      </c>
-      <c r="D15" s="1">
-        <f t="shared" si="1"/>
         <v>468</v>
       </c>
       <c r="E15" s="22">
         <v>697.94299999999998</v>
       </c>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="8">
-        <f t="shared" si="2"/>
+      <c r="F15" s="23">
+        <f>E15/1000</f>
         <v>0.69794299999999998</v>
       </c>
-      <c r="I15" s="1">
-        <f t="shared" si="3"/>
+      <c r="G15" s="1">
+        <f t="shared" si="1"/>
         <v>1.4288009999999999E-3</v>
       </c>
-      <c r="J15" s="2"/>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A16" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="21">
         <v>14</v>
       </c>
       <c r="C16" s="1">
+        <f>B16*$J$5</f>
+        <v>8.4</v>
+      </c>
+      <c r="D16" s="1">
         <f t="shared" si="0"/>
-        <v>8.4</v>
-      </c>
-      <c r="D16" s="1">
-        <f t="shared" si="1"/>
         <v>504</v>
       </c>
       <c r="E16" s="22">
         <v>1428.8009999999999</v>
       </c>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="8">
-        <f t="shared" si="2"/>
+      <c r="F16" s="23">
+        <f>E16/1000</f>
         <v>1.428801</v>
       </c>
-      <c r="I16" s="1">
-        <f t="shared" si="3"/>
+      <c r="G16" s="1">
+        <f t="shared" si="1"/>
         <v>1.272979E-3</v>
       </c>
-      <c r="J16" s="2"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="21">
         <v>15</v>
       </c>
       <c r="C17" s="1">
+        <f>B17*$J$5</f>
+        <v>9</v>
+      </c>
+      <c r="D17" s="1">
         <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="D17" s="1">
-        <f t="shared" si="1"/>
         <v>540</v>
       </c>
       <c r="E17" s="22">
         <v>1272.979</v>
       </c>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="8">
-        <f t="shared" si="2"/>
+      <c r="F17" s="23">
+        <f>E17/1000</f>
         <v>1.2729790000000001</v>
       </c>
-      <c r="I17" s="1">
-        <f t="shared" si="3"/>
+      <c r="G17" s="1">
+        <f t="shared" si="1"/>
         <v>1.434137E-3</v>
       </c>
-      <c r="J17" s="2"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="21">
         <v>16</v>
       </c>
       <c r="C18" s="1">
+        <f>B18*$J$5</f>
+        <v>9.6</v>
+      </c>
+      <c r="D18" s="1">
         <f t="shared" si="0"/>
-        <v>9.6</v>
-      </c>
-      <c r="D18" s="1">
-        <f t="shared" si="1"/>
         <v>576</v>
       </c>
       <c r="E18" s="22">
         <v>1434.1369999999999</v>
       </c>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="8">
-        <f t="shared" si="2"/>
+      <c r="F18" s="23">
+        <f>E18/1000</f>
         <v>1.434137</v>
       </c>
-      <c r="I18" s="1">
-        <f t="shared" si="3"/>
+      <c r="G18" s="1">
+        <f t="shared" si="1"/>
         <v>1.3246710000000001E-3</v>
       </c>
-      <c r="J18" s="2"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="21">
         <v>17</v>
       </c>
       <c r="C19" s="1">
+        <f>B19*$J$5</f>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="D19" s="1">
         <f t="shared" si="0"/>
-        <v>10.199999999999999</v>
-      </c>
-      <c r="D19" s="1">
-        <f t="shared" si="1"/>
         <v>612</v>
       </c>
       <c r="E19" s="22">
         <v>1324.671</v>
       </c>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="8">
-        <f t="shared" si="2"/>
+      <c r="F19" s="23">
+        <f>E19/1000</f>
         <v>1.3246710000000002</v>
       </c>
-      <c r="I19" s="1">
-        <f t="shared" si="3"/>
+      <c r="G19" s="1">
+        <f t="shared" si="1"/>
         <v>9.1704799999999995E-4</v>
       </c>
-      <c r="J19" s="2"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="21">
         <v>18</v>
       </c>
       <c r="C20" s="1">
+        <f>B20*$J$5</f>
+        <v>10.799999999999999</v>
+      </c>
+      <c r="D20" s="1">
         <f t="shared" si="0"/>
-        <v>10.799999999999999</v>
-      </c>
-      <c r="D20" s="1">
-        <f t="shared" si="1"/>
         <v>647.99999999999989</v>
       </c>
       <c r="E20" s="22">
         <v>917.048</v>
       </c>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="8">
-        <f t="shared" si="2"/>
+      <c r="F20" s="23">
+        <f>E20/1000</f>
         <v>0.91704799999999997</v>
       </c>
-      <c r="I20" s="1">
-        <f t="shared" si="3"/>
+      <c r="G20" s="1">
+        <f t="shared" si="1"/>
         <v>6.3300699999999999E-4</v>
       </c>
-      <c r="J20" s="2"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="21">
         <v>19</v>
       </c>
       <c r="C21" s="1">
+        <f>B21*$J$5</f>
+        <v>11.4</v>
+      </c>
+      <c r="D21" s="1">
         <f t="shared" si="0"/>
-        <v>11.4</v>
-      </c>
-      <c r="D21" s="1">
-        <f t="shared" si="1"/>
         <v>684</v>
       </c>
       <c r="E21" s="22">
         <v>633.00699999999995</v>
       </c>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="8">
-        <f t="shared" si="2"/>
+      <c r="F21" s="23">
+        <f>E21/1000</f>
         <v>0.63300699999999999</v>
       </c>
-      <c r="I21" s="1">
-        <f t="shared" si="3"/>
+      <c r="G21" s="1">
+        <f t="shared" si="1"/>
         <v>3.05975E-4</v>
       </c>
-      <c r="J21" s="2"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="21">
         <v>20</v>
       </c>
       <c r="C22" s="1">
+        <f>B22*$J$5</f>
+        <v>12</v>
+      </c>
+      <c r="D22" s="1">
         <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="D22" s="1">
-        <f t="shared" si="1"/>
         <v>720</v>
       </c>
       <c r="E22" s="22">
         <v>305.97500000000002</v>
       </c>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="8">
-        <f t="shared" si="2"/>
+      <c r="F22" s="23">
+        <f>E22/1000</f>
         <v>0.305975</v>
       </c>
-      <c r="I22" s="1">
-        <f t="shared" si="3"/>
+      <c r="G22" s="1">
+        <f t="shared" si="1"/>
         <v>1.20835E-4</v>
       </c>
-      <c r="J22" s="2"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="21">
         <v>21</v>
       </c>
       <c r="C23" s="1">
+        <f>B23*$J$5</f>
+        <v>12.6</v>
+      </c>
+      <c r="D23" s="1">
         <f t="shared" si="0"/>
-        <v>12.6</v>
-      </c>
-      <c r="D23" s="1">
-        <f t="shared" si="1"/>
         <v>756</v>
       </c>
       <c r="E23" s="22">
         <v>120.83499999999999</v>
       </c>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="8">
-        <f t="shared" si="2"/>
+      <c r="F23" s="23">
+        <f>E23/1000</f>
         <v>0.120835</v>
       </c>
-      <c r="I23" s="1">
-        <f t="shared" si="3"/>
+      <c r="G23" s="1">
+        <f t="shared" si="1"/>
         <v>3.9109999999999997E-5</v>
       </c>
-      <c r="J23" s="2"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24" s="21">
         <v>22</v>
       </c>
       <c r="C24" s="1">
+        <f>B24*$J$5</f>
+        <v>13.2</v>
+      </c>
+      <c r="D24" s="1">
         <f t="shared" si="0"/>
-        <v>13.2</v>
-      </c>
-      <c r="D24" s="1">
-        <f t="shared" si="1"/>
         <v>792</v>
       </c>
       <c r="E24" s="22">
         <v>39.11</v>
       </c>
-      <c r="F24" s="22"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="8">
-        <f t="shared" si="2"/>
+      <c r="F24" s="23">
+        <f>E24/1000</f>
         <v>3.9109999999999999E-2</v>
       </c>
-      <c r="I24" s="1">
-        <f t="shared" si="3"/>
+      <c r="G24" s="1">
+        <f t="shared" si="1"/>
         <v>1.5946999999999998E-5</v>
       </c>
-      <c r="J24" s="2"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="21">
         <v>23</v>
       </c>
       <c r="C25" s="1">
+        <f>B25*$J$5</f>
+        <v>13.799999999999999</v>
+      </c>
+      <c r="D25" s="1">
         <f t="shared" si="0"/>
-        <v>13.799999999999999</v>
-      </c>
-      <c r="D25" s="1">
-        <f t="shared" si="1"/>
         <v>827.99999999999989</v>
       </c>
       <c r="E25" s="22">
         <v>15.946999999999999</v>
       </c>
-      <c r="F25" s="22"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="8">
-        <f t="shared" si="2"/>
+      <c r="F25" s="23">
+        <f>E25/1000</f>
         <v>1.5946999999999999E-2</v>
       </c>
-      <c r="I25" s="1">
-        <f t="shared" si="3"/>
+      <c r="G25" s="1">
+        <f t="shared" si="1"/>
         <v>7.9260000000000017E-6</v>
       </c>
-      <c r="J25" s="2"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="21">
         <v>24</v>
       </c>
       <c r="C26" s="1">
+        <f>B26*$J$5</f>
+        <v>14.399999999999999</v>
+      </c>
+      <c r="D26" s="1">
         <f t="shared" si="0"/>
-        <v>14.399999999999999</v>
-      </c>
-      <c r="D26" s="1">
-        <f t="shared" si="1"/>
         <v>863.99999999999989</v>
       </c>
       <c r="E26" s="22">
         <v>7.9260000000000002</v>
       </c>
-      <c r="F26" s="22"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="8">
-        <f t="shared" si="2"/>
+      <c r="F26" s="23">
+        <f>E26/1000</f>
         <v>7.9260000000000008E-3</v>
       </c>
-      <c r="I26" s="1">
-        <f t="shared" si="3"/>
+      <c r="G26" s="1">
+        <f t="shared" si="1"/>
         <v>5.5690000000000004E-6</v>
       </c>
-      <c r="J26" s="2"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B27" s="25">
         <v>25</v>
       </c>
       <c r="C27" s="1">
+        <f>B27*$J$5</f>
+        <v>15</v>
+      </c>
+      <c r="D27" s="4">
         <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="D27" s="4">
-        <f t="shared" si="1"/>
         <v>900</v>
       </c>
       <c r="E27" s="22">
         <v>5.569</v>
       </c>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="8">
-        <f t="shared" si="2"/>
+      <c r="F27" s="23">
+        <f>E27/1000</f>
         <v>5.5690000000000002E-3</v>
       </c>
-      <c r="I27" s="1">
-        <f t="shared" si="3"/>
+      <c r="G27" s="1">
+        <f t="shared" si="1"/>
         <v>4.5750000000000002E-6</v>
       </c>
-      <c r="J27" s="2"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B28" s="1">
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="21">
         <v>26</v>
       </c>
       <c r="C28" s="1">
-        <f t="shared" ref="C28:C33" si="4">B28*$L$5</f>
+        <f t="shared" ref="C28:C33" si="2">B28*$J$5</f>
         <v>15.6</v>
       </c>
       <c r="D28" s="1">
-        <f t="shared" ref="D28:D33" si="5">C28*60</f>
+        <f t="shared" ref="D28:D33" si="3">C28*60</f>
         <v>936</v>
       </c>
       <c r="E28" s="22">
         <v>4.5750000000000002</v>
       </c>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="8">
+      <c r="F28" s="23">
+        <f>E28/1000</f>
+        <v>4.5750000000000001E-3</v>
+      </c>
+      <c r="G28" s="1">
+        <f t="shared" si="1"/>
+        <v>4.8100000000000005E-6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="21">
+        <v>27</v>
+      </c>
+      <c r="C29" s="1">
         <f t="shared" si="2"/>
-        <v>4.5750000000000001E-3</v>
-      </c>
-      <c r="I28" s="1">
+        <v>16.2</v>
+      </c>
+      <c r="D29" s="1">
         <f t="shared" si="3"/>
-        <v>4.8100000000000005E-6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B29" s="1">
-        <v>27</v>
-      </c>
-      <c r="C29" s="1">
-        <f t="shared" si="4"/>
-        <v>16.2</v>
-      </c>
-      <c r="D29" s="1">
-        <f t="shared" si="5"/>
         <v>972</v>
       </c>
       <c r="E29" s="22">
         <v>4.8099999999999996</v>
       </c>
-      <c r="F29" s="22"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="8">
+      <c r="F29" s="23">
+        <f>E29/1000</f>
+        <v>4.81E-3</v>
+      </c>
+      <c r="G29" s="1">
+        <f t="shared" si="1"/>
+        <v>4.9230000000000001E-6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="21">
+        <v>28</v>
+      </c>
+      <c r="C30" s="1">
         <f t="shared" si="2"/>
-        <v>4.81E-3</v>
-      </c>
-      <c r="I29" s="1">
+        <v>16.8</v>
+      </c>
+      <c r="D30" s="1">
         <f t="shared" si="3"/>
-        <v>4.9230000000000001E-6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B30" s="1">
-        <v>28</v>
-      </c>
-      <c r="C30" s="1">
-        <f t="shared" si="4"/>
-        <v>16.8</v>
-      </c>
-      <c r="D30" s="1">
-        <f t="shared" si="5"/>
         <v>1008</v>
       </c>
       <c r="E30" s="22">
         <v>4.923</v>
       </c>
-      <c r="F30" s="22"/>
-      <c r="G30" s="22"/>
-      <c r="H30" s="8">
+      <c r="F30" s="23">
+        <f>E30/1000</f>
+        <v>4.9230000000000003E-3</v>
+      </c>
+      <c r="G30" s="1">
+        <f t="shared" si="1"/>
+        <v>3.5880000000000002E-5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" s="21">
+        <v>29</v>
+      </c>
+      <c r="C31" s="1">
         <f t="shared" si="2"/>
-        <v>4.9230000000000003E-3</v>
-      </c>
-      <c r="I30" s="1">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="D31" s="1">
         <f t="shared" si="3"/>
-        <v>3.5880000000000002E-5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B31" s="1">
-        <v>29</v>
-      </c>
-      <c r="C31" s="1">
-        <f t="shared" si="4"/>
-        <v>17.399999999999999</v>
-      </c>
-      <c r="D31" s="1">
-        <f t="shared" si="5"/>
         <v>1044</v>
       </c>
       <c r="E31" s="22">
         <v>35.880000000000003</v>
       </c>
-      <c r="F31" s="22"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="8">
+      <c r="F31" s="23">
+        <f>E31/1000</f>
+        <v>3.5880000000000002E-2</v>
+      </c>
+      <c r="G31" s="1">
+        <f t="shared" si="1"/>
+        <v>3.6410000000000004E-6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" s="21">
+        <v>30</v>
+      </c>
+      <c r="C32" s="1">
         <f t="shared" si="2"/>
-        <v>3.5880000000000002E-2</v>
-      </c>
-      <c r="I31" s="1">
+        <v>18</v>
+      </c>
+      <c r="D32" s="1">
         <f t="shared" si="3"/>
-        <v>3.6410000000000004E-6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B32" s="1">
-        <v>30</v>
-      </c>
-      <c r="C32" s="1">
-        <f t="shared" si="4"/>
-        <v>18</v>
-      </c>
-      <c r="D32" s="1">
-        <f t="shared" si="5"/>
         <v>1080</v>
       </c>
       <c r="E32" s="22">
         <v>3.641</v>
       </c>
-      <c r="F32" s="22"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="8">
+      <c r="F32" s="23">
+        <f>E32/1000</f>
+        <v>3.6410000000000001E-3</v>
+      </c>
+      <c r="G32" s="1">
+        <f t="shared" si="1"/>
+        <v>4.1160000000000001E-6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B33" s="21">
+        <v>31</v>
+      </c>
+      <c r="C33" s="1">
         <f t="shared" si="2"/>
-        <v>3.6410000000000001E-3</v>
-      </c>
-      <c r="I32" s="1">
+        <v>18.599999999999998</v>
+      </c>
+      <c r="D33" s="1">
         <f t="shared" si="3"/>
-        <v>4.1160000000000001E-6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B33" s="1">
-        <v>31</v>
-      </c>
-      <c r="C33" s="1">
-        <f t="shared" si="4"/>
-        <v>18.599999999999998</v>
-      </c>
-      <c r="D33" s="1">
-        <f t="shared" si="5"/>
         <v>1115.9999999999998</v>
       </c>
-      <c r="E33" s="23">
+      <c r="E33" s="22">
         <v>4.1159999999999997</v>
       </c>
-      <c r="F33" s="25"/>
-      <c r="G33" s="25"/>
-      <c r="H33" s="8">
-        <f t="shared" si="2"/>
+      <c r="F33" s="23">
+        <f>E33/1000</f>
         <v>4.1159999999999999E-3</v>
       </c>
-      <c r="I33" s="1">
-        <f t="shared" si="3"/>
+      <c r="G33" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
-      <c r="G43" s="6"/>
-      <c r="H43" s="6"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
-      <c r="H44" s="6"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
-      <c r="H45" s="6"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
-      <c r="H46" s="6"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
-      <c r="G47" s="6"/>
-      <c r="H47" s="6"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
-      <c r="G48" s="6"/>
-      <c r="H48" s="6"/>
     </row>
     <row r="49" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E49" s="6"/>

</xml_diff>